<commit_message>
finished project, started potential FA project
</commit_message>
<xml_diff>
--- a/data/AAMEHS Data Dictionary.xlsx
+++ b/data/AAMEHS Data Dictionary.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\_Columbia\Analytic EHS\AAMEHS Final Project Group Folder\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\_Columbia\Advanced GIS\agis_final_project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AB8ACD2-C5AE-464F-9088-AD0B3C537E95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DD90C1B-A7F4-486C-AFB1-18C2CAB937BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-9630" yWindow="-12795" windowWidth="22560" windowHeight="11475" xr2:uid="{DD1C3845-3E96-4390-86F7-9505C1EE22A4}"/>
+    <workbookView xWindow="-11595" yWindow="-13275" windowWidth="23010" windowHeight="12360" xr2:uid="{DD1C3845-3E96-4390-86F7-9505C1EE22A4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="117">
   <si>
     <t>Employment</t>
   </si>
@@ -375,6 +375,18 @@
   </si>
   <si>
     <t>number of live births</t>
+  </si>
+  <si>
+    <t>teen_birth</t>
+  </si>
+  <si>
+    <t>geriatric_birth</t>
+  </si>
+  <si>
+    <t>proportion of births with maternal age 15-19</t>
+  </si>
+  <si>
+    <t>proportion of births with maternal age 35+</t>
   </si>
 </sst>
 </file>
@@ -752,10 +764,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7B84DA5-EEEA-4692-AAAB-7F572B9375B0}">
-  <dimension ref="A1:E47"/>
+  <dimension ref="A1:E49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -990,109 +1002,109 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>7</v>
+        <v>113</v>
       </c>
       <c r="B14" t="s">
         <v>47</v>
       </c>
       <c r="C14" t="s">
-        <v>0</v>
+        <v>68</v>
       </c>
       <c r="D14" t="s">
-        <v>46</v>
+        <v>72</v>
       </c>
       <c r="E14" t="s">
-        <v>74</v>
+        <v>115</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>8</v>
+        <v>114</v>
       </c>
       <c r="B15" t="s">
         <v>47</v>
       </c>
       <c r="C15" t="s">
-        <v>0</v>
+        <v>68</v>
       </c>
       <c r="D15" t="s">
-        <v>46</v>
+        <v>72</v>
       </c>
       <c r="E15" t="s">
-        <v>75</v>
+        <v>116</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B16" t="s">
         <v>47</v>
       </c>
       <c r="C16" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D16" t="s">
         <v>46</v>
       </c>
       <c r="E16" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B17" t="s">
         <v>47</v>
       </c>
       <c r="C17" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D17" t="s">
         <v>46</v>
       </c>
       <c r="E17" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B18" t="s">
         <v>47</v>
       </c>
       <c r="C18" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D18" t="s">
         <v>46</v>
       </c>
       <c r="E18" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B19" t="s">
         <v>47</v>
       </c>
       <c r="C19" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D19" t="s">
         <v>46</v>
       </c>
       <c r="E19" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B20" t="s">
         <v>47</v>
@@ -1104,46 +1116,46 @@
         <v>46</v>
       </c>
       <c r="E20" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B21" t="s">
         <v>47</v>
       </c>
       <c r="C21" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D21" t="s">
         <v>46</v>
       </c>
       <c r="E21" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B22" t="s">
         <v>47</v>
       </c>
       <c r="C22" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D22" t="s">
         <v>46</v>
       </c>
       <c r="E22" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B23" t="s">
         <v>47</v>
@@ -1155,12 +1167,12 @@
         <v>46</v>
       </c>
       <c r="E23" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B24" t="s">
         <v>47</v>
@@ -1172,12 +1184,12 @@
         <v>46</v>
       </c>
       <c r="E24" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B25" t="s">
         <v>47</v>
@@ -1189,12 +1201,12 @@
         <v>46</v>
       </c>
       <c r="E25" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B26" t="s">
         <v>47</v>
@@ -1206,12 +1218,12 @@
         <v>46</v>
       </c>
       <c r="E26" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B27" t="s">
         <v>47</v>
@@ -1223,12 +1235,12 @@
         <v>46</v>
       </c>
       <c r="E27" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B28" t="s">
         <v>47</v>
@@ -1240,12 +1252,12 @@
         <v>46</v>
       </c>
       <c r="E28" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B29" t="s">
         <v>47</v>
@@ -1257,46 +1269,46 @@
         <v>46</v>
       </c>
       <c r="E29" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B30" t="s">
         <v>47</v>
       </c>
       <c r="C30" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D30" t="s">
         <v>46</v>
       </c>
       <c r="E30" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B31" t="s">
         <v>47</v>
       </c>
       <c r="C31" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D31" t="s">
         <v>46</v>
       </c>
       <c r="E31" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B32" t="s">
         <v>47</v>
@@ -1308,12 +1320,12 @@
         <v>46</v>
       </c>
       <c r="E32" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B33" t="s">
         <v>47</v>
@@ -1325,12 +1337,12 @@
         <v>46</v>
       </c>
       <c r="E33" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B34" t="s">
         <v>47</v>
@@ -1342,46 +1354,46 @@
         <v>46</v>
       </c>
       <c r="E34" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B35" t="s">
         <v>47</v>
       </c>
       <c r="C35" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D35" t="s">
         <v>46</v>
       </c>
       <c r="E35" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B36" t="s">
         <v>47</v>
       </c>
       <c r="C36" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D36" t="s">
         <v>46</v>
       </c>
       <c r="E36" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B37" t="s">
         <v>47</v>
@@ -1393,12 +1405,12 @@
         <v>46</v>
       </c>
       <c r="E37" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B38" t="s">
         <v>47</v>
@@ -1410,12 +1422,12 @@
         <v>46</v>
       </c>
       <c r="E38" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B39" t="s">
         <v>47</v>
@@ -1427,12 +1439,12 @@
         <v>46</v>
       </c>
       <c r="E39" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B40" t="s">
         <v>47</v>
@@ -1444,12 +1456,12 @@
         <v>46</v>
       </c>
       <c r="E40" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B41" t="s">
         <v>47</v>
@@ -1461,12 +1473,12 @@
         <v>46</v>
       </c>
       <c r="E41" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B42" t="s">
         <v>47</v>
@@ -1478,46 +1490,46 @@
         <v>46</v>
       </c>
       <c r="E42" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B43" t="s">
         <v>47</v>
       </c>
       <c r="C43" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D43" t="s">
         <v>46</v>
       </c>
       <c r="E43" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B44" t="s">
         <v>47</v>
       </c>
       <c r="C44" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D44" t="s">
         <v>46</v>
       </c>
       <c r="E44" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B45" t="s">
         <v>47</v>
@@ -1529,12 +1541,12 @@
         <v>46</v>
       </c>
       <c r="E45" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B46" t="s">
         <v>47</v>
@@ -1546,12 +1558,12 @@
         <v>46</v>
       </c>
       <c r="E46" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B47" t="s">
         <v>47</v>
@@ -1563,6 +1575,40 @@
         <v>46</v>
       </c>
       <c r="E47" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>39</v>
+      </c>
+      <c r="B48" t="s">
+        <v>47</v>
+      </c>
+      <c r="C48" t="s">
+        <v>6</v>
+      </c>
+      <c r="D48" t="s">
+        <v>46</v>
+      </c>
+      <c r="E48" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>40</v>
+      </c>
+      <c r="B49" t="s">
+        <v>47</v>
+      </c>
+      <c r="C49" t="s">
+        <v>6</v>
+      </c>
+      <c r="D49" t="s">
+        <v>46</v>
+      </c>
+      <c r="E49" t="s">
         <v>107</v>
       </c>
     </row>

</xml_diff>